<commit_message>
switching to 2019 PD and adapted portfolio data
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DB226A8-2C44-43FE-97B9-074332171257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB64396-F417-4A0B-A06A-C363A8ED6DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="127">
   <si>
     <t>Setting</t>
   </si>
@@ -412,6 +412,12 @@
   </si>
   <si>
     <t>sub_area_1</t>
+  </si>
+  <si>
+    <t>Tech10</t>
+  </si>
+  <si>
+    <t>Nuclear_adv</t>
   </si>
 </sst>
 </file>
@@ -613,7 +619,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
@@ -625,9 +631,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -663,9 +668,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="11">
     <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
     <cellStyle name="Comma 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Currency 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -677,7 +681,6 @@
     <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 5" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21"/>
-    <cellStyle name="Percent" xfId="11" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1014,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BD10"/>
+  <dimension ref="A1:BD6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:I18"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1225,7 +1228,7 @@
         <v>69</v>
       </c>
       <c r="I2">
-        <v>309</v>
+        <v>343</v>
       </c>
       <c r="J2" s="9">
         <v>100</v>
@@ -1309,7 +1312,7 @@
         <v>74</v>
       </c>
       <c r="I3">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J3" s="9">
         <v>100</v>
@@ -1375,13 +1378,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>77</v>
@@ -1393,7 +1396,7 @@
         <v>77</v>
       </c>
       <c r="I4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J4" s="9">
         <v>1000</v>
@@ -1477,7 +1480,7 @@
         <v>88</v>
       </c>
       <c r="I5">
-        <v>193</v>
+        <v>250</v>
       </c>
       <c r="J5" s="9">
         <v>200</v>
@@ -1561,7 +1564,7 @@
         <v>88</v>
       </c>
       <c r="I6">
-        <v>429</v>
+        <v>508</v>
       </c>
       <c r="J6" s="9">
         <v>50</v>
@@ -1619,9 +1622,6 @@
       <c r="BC6" s="10"/>
       <c r="BD6" s="10"/>
     </row>
-    <row r="10" spans="1:56">
-      <c r="I10" s="15"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reverting to 250 NG units to avoid period-2 infeasibility
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB64396-F417-4A0B-A06A-C363A8ED6DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEBF07E-F428-4BF7-90F2-F3407CC73443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:BD6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
final versions of inputs with data values producing sensible results/no infeasibility conditions
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEBF07E-F428-4BF7-90F2-F3407CC73443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72205359-3FAB-4505-ABEF-6D24ECE6AC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1480,7 +1480,7 @@
         <v>88</v>
       </c>
       <c r="I5">
-        <v>250</v>
+        <v>280</v>
       </c>
       <c r="J5" s="9">
         <v>200</v>

</xml_diff>

<commit_message>
updating settings and data
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72205359-3FAB-4505-ABEF-6D24ECE6AC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFAB955-42BA-4941-84C8-6FCC98D85DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1017,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BD6"/>
+  <dimension ref="A1:BD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1370,36 +1370,36 @@
       <c r="BC3" s="10"/>
       <c r="BD3" s="10"/>
     </row>
-    <row r="4" spans="1:56">
+    <row r="4" spans="1:56" customFormat="1">
       <c r="A4" s="6" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>280</v>
       </c>
       <c r="J4" s="9">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="K4" s="12">
         <v>99999999</v>
@@ -1454,36 +1454,36 @@
       <c r="BC4" s="10"/>
       <c r="BD4" s="10"/>
     </row>
-    <row r="5" spans="1:56">
+    <row r="5" spans="1:56" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>88</v>
       </c>
       <c r="I5">
-        <v>280</v>
+        <v>508</v>
       </c>
       <c r="J5" s="9">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="K5" s="12">
         <v>99999999</v>
@@ -1538,36 +1538,36 @@
       <c r="BC5" s="10"/>
       <c r="BD5" s="10"/>
     </row>
-    <row r="6" spans="1:56">
+    <row r="6" spans="1:56" customFormat="1">
       <c r="A6" s="6" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="I6">
-        <v>508</v>
+        <v>17</v>
       </c>
       <c r="J6" s="9">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="K6" s="12">
         <v>99999999</v>
@@ -1622,6 +1622,7 @@
       <c r="BC6" s="10"/>
       <c r="BD6" s="10"/>
     </row>
+    <row r="7" spans="1:56" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleanup to input files
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFAB955-42BA-4941-84C8-6FCC98D85DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F390A3-3169-40BA-91F9-00AC1939FB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1017,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BD7"/>
+  <dimension ref="A1:BD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1370,7 +1370,7 @@
       <c r="BC3" s="10"/>
       <c r="BD3" s="10"/>
     </row>
-    <row r="4" spans="1:56" customFormat="1">
+    <row r="4" spans="1:56">
       <c r="A4" s="6" t="s">
         <v>83</v>
       </c>
@@ -1454,7 +1454,7 @@
       <c r="BC4" s="10"/>
       <c r="BD4" s="10"/>
     </row>
-    <row r="5" spans="1:56" customFormat="1">
+    <row r="5" spans="1:56">
       <c r="A5" s="6" t="s">
         <v>89</v>
       </c>
@@ -1538,7 +1538,7 @@
       <c r="BC5" s="10"/>
       <c r="BD5" s="10"/>
     </row>
-    <row r="6" spans="1:56" customFormat="1">
+    <row r="6" spans="1:56">
       <c r="A6" s="6" t="s">
         <v>75</v>
       </c>
@@ -1622,7 +1622,6 @@
       <c r="BC6" s="10"/>
       <c r="BD6" s="10"/>
     </row>
-    <row r="7" spans="1:56" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changing 'UNIT_TYPE' and 'Unit Type' columns to hold the standardized, descriptive unit type names for ABCE
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_ERCOT_5units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F390A3-3169-40BA-91F9-00AC1939FB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830133BA-4533-481E-9817-C5B47B052374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="128">
   <si>
     <t>Setting</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Nuclear_adv</t>
+  </si>
+  <si>
+    <t>AdvancedNuclear</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1023,7 @@
   <dimension ref="A1:BD6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1306,7 +1309,7 @@
         <v>73</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>74</v>
@@ -1390,7 +1393,7 @@
         <v>86</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>88</v>
@@ -1474,7 +1477,7 @@
         <v>92</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>88</v>
@@ -1558,7 +1561,7 @@
         <v>77</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>77</v>

</xml_diff>